<commit_message>
Hielprik Algemeen extra dingen toegevoegd
</commit_message>
<xml_diff>
--- a/src/main/resources/nhs-dmn/OriginelenVoorBusiness/hpa_HielprikAlgemeenOrigineel.xlsx
+++ b/src/main/resources/nhs-dmn/OriginelenVoorBusiness/hpa_HielprikAlgemeenOrigineel.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\han\git\rivm\nhs\dmn\nhs-business\src\main\resources\nhs-dmn\OriginelenVoorBusiness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC50F8F3-A531-4D4C-9C5E-16C2D4F17720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A09C3BE-EFD4-42CB-8C81-B90DFB9BC742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="834" activeTab="1" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
+    <workbookView xWindow="4515" yWindow="2355" windowWidth="21900" windowHeight="13050" tabRatio="834" activeTab="5" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
   </bookViews>
   <sheets>
     <sheet name="Lijstjes" sheetId="7" r:id="rId1"/>
-    <sheet name="Status BT" sheetId="15" r:id="rId2"/>
+    <sheet name="status BT" sheetId="15" r:id="rId2"/>
     <sheet name="isTweedeHielprik" sheetId="24" r:id="rId3"/>
     <sheet name="isPrematuur" sheetId="13" r:id="rId4"/>
     <sheet name="isTeVroegGeprikt" sheetId="4" r:id="rId5"/>
+    <sheet name="voldoendeTijdVerstrekenBT" sheetId="25" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">isPrematuur!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">isTweedeHielprik!$A$1:$B$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Status BT'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'status BT'!$A$1:$D$1</definedName>
     <definedName name="ActieBTwaarden">Lijstjes!$C$2:$C$6</definedName>
     <definedName name="ActieCodeWaarden">Lijstjes!$D$2:$D$10</definedName>
     <definedName name="AfnameTermijnVeld">Lijstjes!$L$2:$L$4</definedName>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="122">
   <si>
     <t>Interpretatie</t>
   </si>
@@ -237,15 +238,9 @@
     <t>&gt; -3.0</t>
   </si>
   <si>
-    <t>afname - geboorte</t>
-  </si>
-  <si>
     <t>&gt;= 48</t>
   </si>
   <si>
-    <t>AfnameTijd EN GeboorteTijd bekend?</t>
-  </si>
-  <si>
     <t>&gt;= 72</t>
   </si>
   <si>
@@ -420,10 +415,22 @@
     <t>Actie_BT</t>
   </si>
   <si>
-    <t>VoldoendeTijdVerstrekenBT</t>
-  </si>
-  <si>
-    <t>Status BT</t>
+    <t>(hielprik.afnameMoment - hielprik.geboorteMoment).hours</t>
+  </si>
+  <si>
+    <t>(hielprik.afnameMoment - hielprik.bloedtransfusieMoment).hours</t>
+  </si>
+  <si>
+    <t>voldoendeTijdVerstrekenBT</t>
+  </si>
+  <si>
+    <t>status BT</t>
+  </si>
+  <si>
+    <t>(time(hielprik.afnameMoment) = time(0,0,0)) and (time(hielprik.geboorteMoment) = time(0,0,0))</t>
+  </si>
+  <si>
+    <t>(time(hielprik.afnameMoment) = time(0,0,0)) and (time(hielprik.bloedtransfusieMoment) = time(0,0,0))</t>
   </si>
 </sst>
 </file>
@@ -564,7 +571,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -572,7 +579,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -582,11 +588,20 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -942,25 +957,25 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D1" t="s">
         <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" t="s">
         <v>107</v>
-      </c>
-      <c r="H1" t="s">
-        <v>108</v>
-      </c>
-      <c r="I1" t="s">
-        <v>109</v>
       </c>
       <c r="J1" t="s">
         <v>1</v>
@@ -993,13 +1008,13 @@
         <v>4</v>
       </c>
       <c r="T1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="U1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="V1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -1010,22 +1025,22 @@
         <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I2" t="s">
         <v>38</v>
@@ -1067,7 +1082,7 @@
         <v>38</v>
       </c>
       <c r="V2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -1078,22 +1093,22 @@
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I3" t="s">
         <v>40</v>
@@ -1117,7 +1132,7 @@
         <v>23</v>
       </c>
       <c r="P3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q3" t="s">
         <v>26</v>
@@ -1129,13 +1144,13 @@
         <v>31</v>
       </c>
       <c r="T3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="U3" t="s">
         <v>39</v>
       </c>
       <c r="V3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -1146,25 +1161,25 @@
         <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J4" t="s">
         <v>49</v>
@@ -1185,7 +1200,7 @@
         <v>19</v>
       </c>
       <c r="P4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Q4" t="s">
         <v>19</v>
@@ -1203,7 +1218,7 @@
         <v>40</v>
       </c>
       <c r="V4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -1217,7 +1232,7 @@
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
@@ -1226,13 +1241,13 @@
         <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H5" t="s">
+        <v>108</v>
+      </c>
+      <c r="I5" t="s">
         <v>110</v>
-      </c>
-      <c r="I5" t="s">
-        <v>112</v>
       </c>
       <c r="J5" t="s">
         <v>53</v>
@@ -1259,10 +1274,10 @@
         <v>51</v>
       </c>
       <c r="U5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="V5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -1273,7 +1288,7 @@
         <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E6" t="s">
         <v>51</v>
@@ -1309,15 +1324,15 @@
         <v>51</v>
       </c>
       <c r="U6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="V6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G7" t="s">
         <v>19</v>
@@ -1341,15 +1356,15 @@
         <v>29</v>
       </c>
       <c r="U7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="V7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K8" t="s">
         <v>47</v>
@@ -1361,15 +1376,15 @@
         <v>51</v>
       </c>
       <c r="U8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="V8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K9" t="s">
         <v>50</v>
@@ -1383,7 +1398,7 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K10" t="s">
         <v>49</v>
@@ -1420,8 +1435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B88B274-76A9-4F9C-97E3-D90602F3F1BF}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1435,252 +1450,252 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>118</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>88</v>
+      <c r="A3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>115</v>
+      <c r="A4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="F4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>88</v>
+      <c r="A5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="A6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="E8" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="E9" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="E10" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="E11" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="5"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{3B88B274-76A9-4F9C-97E3-D90602F3F1BF}"/>
@@ -1730,41 +1745,41 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B3" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1792,197 +1807,197 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="B7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="6" t="s">
+      <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="C11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="C12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2001,74 +2016,145 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCFCADA8-35EC-4674-BB10-19E37C561E05}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="43.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="43.5703125" style="8"/>
+    <col min="3" max="3" width="21.5703125" style="8" customWidth="1"/>
+    <col min="4" max="16384" width="43.5703125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6089BCB3-59FA-48DD-AFE8-83D4B86AC8DD}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>33</v>
+      <c r="C5" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>